<commit_message>
Modified code and Executed Framework
</commit_message>
<xml_diff>
--- a/Input_Data/Inputs.xlsx
+++ b/Input_Data/Inputs.xlsx
@@ -1,13 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB1180D-CC8A-4110-BA72-D2A178A5B1BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Valid Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Verify Product Version" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +21,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Product Version</t>
+  </si>
+  <si>
+    <t>ErrMsg</t>
+  </si>
+  <si>
+    <t>Username or Password is invalid. Please try again.</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>actiTIME - Enter Time-Track</t>
+  </si>
+  <si>
+    <t>Title of home page</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +86,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +387,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16204378-44D3-40C0-8922-81315AECD870}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C14F377-9034-4D16-898B-EF4D856D1883}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
simply doing commit and push
</commit_message>
<xml_diff>
--- a/Input_Data/Inputs.xlsx
+++ b/Input_Data/Inputs.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB1180D-CC8A-4110-BA72-D2A178A5B1BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{648C8DFF-4AAD-4B4A-8D99-E276C0F56809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15096" windowHeight="4320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid Login" sheetId="1" r:id="rId1"/>
     <sheet name="Invalid Login" sheetId="2" r:id="rId2"/>
     <sheet name="Verify Product Version" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -55,6 +56,9 @@
   </si>
   <si>
     <t>Title of home page</t>
+  </si>
+  <si>
+    <t>actiTIME 2017.4</t>
   </si>
 </sst>
 </file>
@@ -501,10 +505,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -524,8 +532,8 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>123</v>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jenkins was not running so pushing the code again
</commit_message>
<xml_diff>
--- a/Input_Data/Inputs.xlsx
+++ b/Input_Data/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{648C8DFF-4AAD-4B4A-8D99-E276C0F56809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4D8212D1-77C9-49DE-AF19-69E3B3E27A34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15096" windowHeight="4320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15096" windowHeight="5532" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid Login" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Verify Product Version" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:L17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
deleted a class file
</commit_message>
<xml_diff>
--- a/Input_Data/Inputs.xlsx
+++ b/Input_Data/Inputs.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4D8212D1-77C9-49DE-AF19-69E3B3E27A34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15096" windowHeight="5532" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13095" windowHeight="4785" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Valid Login" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="Verify Product Version" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L17"/>
+  <oleSize ref="A1:J14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -207,7 +206,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -384,24 +383,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -432,18 +431,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16204378-44D3-40C0-8922-81315AECD870}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="44.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -501,17 +500,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C14F377-9034-4D16-898B-EF4D856D1883}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implemented scripts for login
</commit_message>
<xml_diff>
--- a/Input_Data/Inputs.xlsx
+++ b/Input_Data/Inputs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13725" windowHeight="4980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12270" windowHeight="4095" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Valid Login" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Verify Product Version" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J15"/>
+  <oleSize ref="A1:I11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -383,7 +383,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,7 +393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>